<commit_message>
update 2 files and create 2 files
</commit_message>
<xml_diff>
--- a/plant/Data diagram.xlsx
+++ b/plant/Data diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\E-Commerce\plant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C90CC76-155A-426D-B1E2-0A68952FECD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625A822D-B8B3-4EC5-8630-015A9411571A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="15040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
   <si>
     <t>User</t>
   </si>
@@ -185,6 +185,42 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>roomId</t>
+  </si>
+  <si>
+    <t>adminId</t>
+  </si>
+  <si>
+    <t>customerId</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>roomId(uuid)</t>
+  </si>
+  <si>
+    <t>senderId</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>wardId</t>
+  </si>
+  <si>
+    <t>provinceId</t>
+  </si>
+  <si>
+    <t>districtId</t>
   </si>
 </sst>
 </file>
@@ -234,9 +270,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:Q42"/>
+  <dimension ref="C4:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -533,21 +570,25 @@
     <col min="17" max="17" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -560,66 +601,81 @@
       <c r="I5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>25</v>
       </c>
@@ -753,11 +809,15 @@
       <c r="C28" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="G28" s="2"/>
+      <c r="I28" s="2"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
         <v>2</v>
       </c>
+      <c r="G29" s="2"/>
+      <c r="I29" s="2"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
@@ -825,6 +885,46 @@
     <row r="42" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>54</v>
+      </c>
+      <c r="E50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>